<commit_message>
logic board change, flipped orientation
Added note about press in threads.
Flipped power connector (polarity might be wrong, but keyed) .
</commit_message>
<xml_diff>
--- a/Hardware/Project Outputs for Heliotrope_Logic/BOM/Bill of Materials-Heliotrope_Logic.xlsx
+++ b/Hardware/Project Outputs for Heliotrope_Logic/BOM/Bill of Materials-Heliotrope_Logic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Altium\Projects\Heliotrope_Logic\Project Outputs for Heliotrope_Logic\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{895EFD8F-0BAD-48F3-98EC-29A394CFC939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C62A2EF-E12F-4BA9-B89F-C024D56A9402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3885" yWindow="2205" windowWidth="28800" windowHeight="15435" xr2:uid="{C60DBC35-51E9-4B57-B467-CC0D5236716B}"/>
+    <workbookView xWindow="3885" yWindow="2205" windowWidth="28800" windowHeight="15435" xr2:uid="{B301855D-F335-4C8B-81FA-01724E6076FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-Heliotrope_Lo" sheetId="1" r:id="rId1"/>
@@ -579,7 +579,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7724875E-4D43-4077-B303-FF09BFDC1B44}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C190744-000D-44B8-8C84-5B18F746285D}">
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>